<commit_message>
commented out sql server code of data manipulation.
</commit_message>
<xml_diff>
--- a/employee_data.xlsx
+++ b/employee_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -487,16 +487,16 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ram</t>
+          <t>Tom</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>people</t>
+          <t>Finance</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -512,74 +512,49 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Tom</t>
+          <t>Sofi</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Finance</t>
+          <t>Sales</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2025-03-09</t>
+          <t>2025-03-10</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2025-03-09</t>
+          <t>2025-03-10</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Sofi</t>
+          <t>Siya</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Sales</t>
+          <t>Data Team</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2025-03-10</t>
+          <t>2025-03-12</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
-        <is>
-          <t>2025-03-10</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>7</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Siya</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Data Team</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>2025-03-12</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
         <is>
           <t>2025-03-12</t>
         </is>

</xml_diff>